<commit_message>
measure & sketch tools fixed
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>Non-Editor QC</t>
+  </si>
+  <si>
+    <t>measure &amp; sketch tools fixed</t>
+  </si>
+  <si>
+    <t>botht eh measure tool and the sketch tool permitted drawing multiple polyline segments and actually included the distances between them when calculating the total measured distance and DE project distance. Added a variable to hold each segment length for the DE tool, set the measure tool to refresh measuring the distance with each line drawn, and created a 'mouse-move' event so that the measured distance fluvially updates with mouse movement.</t>
+  </si>
+  <si>
+    <t>Make multiple segments with each unit type in the Measure tab. DO this both in the current version and this working version of the SPM and compare. Repeat this process in the Sketch Tool tab, making a project with multiple segments very far away from each other to ensure that the total project length doesn't include the gap between the segments</t>
   </si>
 </sst>
 </file>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +561,26 @@
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42269</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed railroad legend/fixed Area Office spelling error/added link to minute orders
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t xml:space="preserve">for each tab in the TOC hover the pointer over all objects and verify that the pointer hand shows up for clickable objects and also does not show up for non-clickabl objects </t>
+  </si>
+  <si>
+    <t>cbardash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed Railroad Legend and Popup to show text descriptions instead of codes.  Replaced railroad service with new service.  Replaced InfoTemplate with PopupTemplate, since InfoTemplates cannot interpret coded domain values.
+Changed Area Office layer to point to new service.  Added District Name to the popup window.
+Added a link in the popup for the Highway Designation layer that points to the Minute Orders page based on the minute order number in the popup.
+</t>
+  </si>
+  <si>
+    <t>see SPM_TestScrip.docx</t>
   </si>
 </sst>
 </file>
@@ -474,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +622,23 @@
         <v>22</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42324</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added area office renderer/fixed RR popup title/removed ESRI logo
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>see SPM_TestScrip.docx</t>
+  </si>
+  <si>
+    <t>11/17/</t>
+  </si>
+  <si>
+    <t>fixed Railroad legend/fixed Area Office misspelling/added link to minute orders</t>
+  </si>
+  <si>
+    <t>Added renderer to Area Office layer to mimic transparency on old layer</t>
   </si>
 </sst>
 </file>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +641,9 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
@@ -639,6 +651,20 @@
         <v>25</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed legend for Clear Overlays/updated MPO layer/updatedHighwayDesignations layer/added highlighter for Search tab
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -99,13 +99,24 @@
     <t>see SPM_TestScrip.docx</t>
   </si>
   <si>
-    <t>11/17/</t>
-  </si>
-  <si>
     <t>fixed Railroad legend/fixed Area Office misspelling/added link to minute orders</t>
   </si>
   <si>
-    <t>Added renderer to Area Office layer to mimic transparency on old layer</t>
+    <t>Added renderer to Area Office layer to mimic transparency on old layer
+Fixed RR popup title
+removed ESRI logo</t>
+  </si>
+  <si>
+    <t>added area office renderer/fixed RR popup title/ removed ESRI logo</t>
+  </si>
+  <si>
+    <t>Fixed "Clear Overlays" legend.
+Added new 2015 MPO Map Service layer and added renderer to handle transparency problem.
+Replaced old service layer for Highway Designations with new Map Service (now includes historic minute orders and has been resymbolized).
+Added highlight function to Search tab.</t>
+  </si>
+  <si>
+    <t>fixed legend for Clear Overlays/updated MPO layer/updatedHighwayDesignations layer/added highlighter for Search tab</t>
   </si>
 </sst>
 </file>
@@ -495,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +653,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>24</v>
@@ -654,17 +665,43 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>42325</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added survey/removed attribution from lower right-hand corner/removed ArcGIS Server layer URLs/added version number
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>fixed legend for Clear Overlays/updated MPO layer/updatedHighwayDesignations layer/added highlighter for Search tab</t>
+  </si>
+  <si>
+    <t>Added survey popup screen on startup, and also survey button at bottom of TOC.
+Removed esriAttribution from lower right-hand corner.
+Switched ArcGIS Server-based services over to AGO-hosted services.
+Added version number to About tab.</t>
+  </si>
+  <si>
+    <t>added survey/removed attribution from lower right-hand corner/removed ArcGIS Server layer URLs/added version number</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +711,26 @@
         <v>25</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
multiple fixes following updates
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -99,13 +99,33 @@
     <t>see SPM_TestScrip.docx</t>
   </si>
   <si>
-    <t>11/17/</t>
-  </si>
-  <si>
     <t>fixed Railroad legend/fixed Area Office misspelling/added link to minute orders</t>
   </si>
   <si>
-    <t>Added renderer to Area Office layer to mimic transparency on old layer</t>
+    <t>Added renderer to Area Office layer to mimic transparency on old layer
+Fixed RR popup title
+removed ESRI logo</t>
+  </si>
+  <si>
+    <t>added area office renderer/fixed RR popup title/ removed ESRI logo</t>
+  </si>
+  <si>
+    <t>Fixed "Clear Overlays" legend.
+Added new 2015 MPO Map Service layer and added renderer to handle transparency problem.
+Replaced old service layer for Highway Designations with new Map Service (now includes historic minute orders and has been resymbolized).
+Added highlight function to Search tab.</t>
+  </si>
+  <si>
+    <t>fixed legend for Clear Overlays/updated MPO layer/updatedHighwayDesignations layer/added highlighter for Search tab</t>
+  </si>
+  <si>
+    <t>Added survey popup screen on startup, and also survey button at bottom of TOC.
+Removed esriAttribution from lower right-hand corner.
+Switched ArcGIS Server-based services over to AGO-hosted services.
+Added version number to About tab.</t>
+  </si>
+  <si>
+    <t>added survey/removed attribution from lower right-hand corner/removed ArcGIS Server layer URLs/added version number</t>
   </si>
 </sst>
 </file>
@@ -495,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +662,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>24</v>
@@ -654,17 +674,63 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>42325</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>42339</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>42352</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated spreadsheet with IDs and version number
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Date</t>
   </si>
@@ -119,13 +119,52 @@
     <t>fixed legend for Clear Overlays/updated MPO layer/updatedHighwayDesignations layer/added highlighter for Search tab</t>
   </si>
   <si>
+    <t>added survey/removed attribution from lower right-hand corner/removed ArcGIS Server layer URLs/added version number</t>
+  </si>
+  <si>
+    <t>multiple fixes following updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple fixes following updates:
+Measure Tab: Fixed problem with other units of measure not populating. Also, first graphic clears now after starting a second.
+Search Tab: Changed the styling of the search results div so that it is only there if there is a result, and then it is only as big as the results. Moved clear button to map below zoom toggle. New button shows up under zoom toggle when a feature is selected.  The button disappears again when clicked. Button is visible on all tabs until the highlighted feature is cleared, so that user doesn’t have to return to Search tab to clear it.  Changed search results message from "Nothing found, Try a new search" to "Searching."
+Fixed credits at bottom right of map pane so that long credits do not show up. Disabled Esri-based credentials and hard-coded credentials to a new div.
+Popups hide when a new Tab or Overlay is selected.
+Query Tab: Comma or letter (anything other than a number) in Value field causes query to run forever. Changed field type to “number.
+Explanation of Control Section colors in legend. Now reads “Control Section Segment colors only serve to distinguish one segment from the next.”
+Repositioned Jump To button and tweak styling to round bottom edge of dropdown.
+Legislative boundary layers: Plan Name field in popup dialog box is always empty.  Field is blank in all three service layers.  Removed field from popup.
+Changed Maintenance Section label in legend to "Maintenance Offices" to be consistant with Overlay title.
+Changed Minute Order Designations title in Legend to Highway Designations to be consistant with Overlay title.
+</t>
+  </si>
+  <si>
+    <t>Testers from this round of major updates all tested these fixes.</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>4.1.1 info</t>
+  </si>
+  <si>
+    <t>44, 43, 41</t>
+  </si>
+  <si>
     <t>Added survey popup screen on startup, and also survey button at bottom of TOC.
 Removed esriAttribution from lower right-hand corner.
 Switched ArcGIS Server-based services over to AGO-hosted services.
-Added version number to About tab.</t>
-  </si>
-  <si>
-    <t>added survey/removed attribution from lower right-hand corner/removed ArcGIS Server layer URLs/added version number</t>
+Added version number to About tab.
+Added Jump to Google/Bing button.</t>
+  </si>
+  <si>
+    <t>50, 27</t>
+  </si>
+  <si>
+    <t>52, 40, 37, 20</t>
   </si>
 </sst>
 </file>
@@ -150,7 +189,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,11 +221,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -196,23 +232,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,223 +557,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="76.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="67" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="76.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="67" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="9.140625" style="11"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="H1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>42265</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4">
+        <v>45</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>42269</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>42269</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>42269</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>42270</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>42324</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="F7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>42325</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>42339</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>42352</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42375</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>10</v>
+      <c r="D11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added meta tag to fix IE problem / Updated Maint Sec layer / added Creative Commons license
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,18 @@
   </si>
   <si>
     <t>52, 40, 37, 20</t>
+  </si>
+  <si>
+    <t>Added meta tag to fix IR problem / Updated Maint Sec layer / added Creative Commones license</t>
+  </si>
+  <si>
+    <t>Meta tag fixes compatibility view problem with IE.  Added new Maintenance Section layer on AGO and updated service.  Added Creative Commons license statement to top.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Open in IE with Compatibility View turned on and check that the app looks correct and all functions work.  Turn on Maintenance Section layer and select polygons to test popup.</t>
   </si>
 </sst>
 </file>
@@ -251,10 +263,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +585,7 @@
     <col min="6" max="6" width="14.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" style="4" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="9.140625" style="11"/>
+    <col min="9" max="9" width="9.140625" style="10"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -631,7 +643,7 @@
       <c r="H2" s="4">
         <v>45</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -648,7 +660,7 @@
       <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -657,7 +669,7 @@
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -674,14 +686,14 @@
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="11"/>
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -707,7 +719,7 @@
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -733,7 +745,7 @@
       <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -762,7 +774,7 @@
       <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -788,7 +800,7 @@
       <c r="G8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -817,7 +829,7 @@
       <c r="H9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -846,7 +858,7 @@
       <c r="H10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>37</v>
       </c>
     </row>
@@ -872,7 +884,33 @@
       <c r="G11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42409</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" s="10" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
4.1.2 Pitt: API 3.16, UZA Layer, 2014 Traffic, Freight, FC Urban/Rural breaks and symbology, Political boundaris, NHS, Top 100, Release Notes
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -194,7 +194,8 @@
 Added a new line in the popup window for FC Linework to show the Rural Code Description
 Updated Political Boundaries and added hyperlinks
 Added Texas Highway Freight Network
-Updated National Highway Freight Network</t>
+Updated National Highway Freight Network
+Updated National Highway Systems Layer</t>
   </si>
 </sst>
 </file>
@@ -589,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
4.1.2 Pitt: API 3.16, 2010 UZA, 2014 AADT, Future Traffic, Top 100, Freight Networks, FC Symbology and Urban/Rural info, Political Boundaries, NHS, Query Function, release notes, excel sheet
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -184,7 +184,7 @@
   <si>
     <t>Added Top 100 Layer with search functionality
 Updated AADT Layer to add 2014 AADT
-Updated the ESRI javascript API to 4.16
+Updated the ESRI javascript API to 3.16
     - this allowed for adding halos around labels
     - required an update to the search functionality
 Updated the Future Traffic and Freight Percentage layer
@@ -195,7 +195,8 @@
 Updated Political Boundaries and added hyperlinks
 Added Texas Highway Freight Network
 Updated National Highway Freight Network
-Updated National Highway Systems Layer</t>
+Updated National Highway Systems Layer
+Updated Query Function to use 2014 Roadway Inventory Data</t>
   </si>
 </sst>
 </file>
@@ -590,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +934,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="240" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
4.1.2 Pitt: API 3.16, 2010 UZA, 2014 AADT, Future Traffic, Top 100, Freight, FC symbology and Urban/Rural info, Political Boundaries, NHS, Query 2014 RI, Project Tracker layer, release notes, excel sheet
</commit_message>
<xml_diff>
--- a/StatewidePlanningMap/SPM_Updates_Performed.xlsx
+++ b/StatewidePlanningMap/SPM_Updates_Performed.xlsx
@@ -196,7 +196,8 @@
 Added Texas Highway Freight Network
 Updated National Highway Freight Network
 Updated National Highway Systems Layer
-Updated Query Function to use 2014 Roadway Inventory Data</t>
+Updated Query Function to use 2014 Roadway Inventory Data
+Updated Projects to Project Tracker layer</t>
   </si>
 </sst>
 </file>
@@ -591,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -934,7 +935,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="240" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="255" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
         <v>47</v>
       </c>

</xml_diff>